<commit_message>
Modifying code for unique structure of PR data.  Major change was using campaign_date to distinguish distinct visits.  Be sure to run renv;;restor() after pulling commit
</commit_message>
<xml_diff>
--- a/inputData/prData_09.20.2023.xlsx
+++ b/inputData/prData_09.20.2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/PRresGHG/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{776D83BB-E38F-49FD-8494-AF8B7AC5CAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{563FD5C5-3858-4FF8-AF5C-5325941EF7FE}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{776D83BB-E38F-49FD-8494-AF8B7AC5CAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4012E15E-E0E0-4898-B8F6-50D3975DAD7F}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm.Database">data!$B$2:$BP$47</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentManualCount="4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="205">
   <si>
     <t>F1</t>
   </si>
@@ -701,9 +701,6 @@
     <t>SG230681</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>11:31</t>
   </si>
   <si>
@@ -720,6 +717,9 @@
   </si>
   <si>
     <t>15:28</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -871,12 +871,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="39">
@@ -1732,78 +1726,78 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W11" sqref="W11"/>
+      <selection pane="topRight" activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.26171875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" customWidth="1"/>
-    <col min="5" max="5" width="13.68359375" customWidth="1"/>
-    <col min="6" max="7" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.26171875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.734375" style="25" customWidth="1"/>
-    <col min="22" max="22" width="16.89453125" customWidth="1"/>
-    <col min="23" max="23" width="13.47265625" customWidth="1"/>
-    <col min="24" max="24" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.3671875" customWidth="1"/>
-    <col min="26" max="26" width="13.89453125" customWidth="1"/>
-    <col min="27" max="27" width="9.26171875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.05078125" customWidth="1"/>
-    <col min="29" max="29" width="7.62890625" customWidth="1"/>
-    <col min="30" max="30" width="10.26171875" customWidth="1"/>
-    <col min="31" max="31" width="6.26171875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" style="25" customWidth="1"/>
+    <col min="22" max="22" width="16.88671875" customWidth="1"/>
+    <col min="23" max="23" width="13.44140625" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" customWidth="1"/>
+    <col min="26" max="26" width="13.88671875" customWidth="1"/>
+    <col min="27" max="27" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" customWidth="1"/>
+    <col min="29" max="29" width="7.6640625" customWidth="1"/>
+    <col min="30" max="30" width="10.21875" customWidth="1"/>
+    <col min="31" max="31" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.68359375" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="9.26171875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.26171875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="7.41796875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.68359375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.68359375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.26171875" customWidth="1"/>
-    <col min="51" max="51" width="8.26171875" customWidth="1"/>
-    <col min="52" max="52" width="10.26171875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="23.26171875" customWidth="1"/>
-    <col min="65" max="65" width="14.83984375" customWidth="1"/>
-    <col min="66" max="66" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.26171875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.21875" customWidth="1"/>
+    <col min="51" max="51" width="8.21875" customWidth="1"/>
+    <col min="52" max="52" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="23.21875" customWidth="1"/>
+    <col min="65" max="65" width="14.88671875" customWidth="1"/>
+    <col min="66" max="66" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="18" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="22.68359375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1889,7 @@
       <c r="BY1" s="31"/>
       <c r="BZ1" s="31"/>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
@@ -2131,7 +2125,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="B3">
         <v>8</v>
       </c>
@@ -2164,7 +2161,7 @@
         <v>182</v>
       </c>
       <c r="U3" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W3">
         <v>25</v>
@@ -2178,7 +2175,10 @@
       <c r="BY3" s="28"/>
       <c r="BZ3" s="26"/>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="B4">
         <v>7</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>182</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="W4">
         <v>23</v>
@@ -2220,7 +2220,10 @@
         <v>32.33</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="B5">
         <v>5</v>
       </c>
@@ -2250,7 +2253,7 @@
         <v>182</v>
       </c>
       <c r="U5" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="W5">
         <v>25</v>
@@ -2262,7 +2265,10 @@
         <v>32.29</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="B6">
         <v>6</v>
       </c>
@@ -2295,7 +2301,7 @@
         <v>182</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="W6">
         <v>25</v>
@@ -2307,7 +2313,10 @@
         <v>32.28</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="B7">
         <v>1</v>
       </c>
@@ -2340,7 +2349,7 @@
         <v>182</v>
       </c>
       <c r="U7" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="W7">
         <v>25</v>
@@ -2352,7 +2361,10 @@
         <v>32.42</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="B8">
         <v>2</v>
       </c>
@@ -2379,7 +2391,7 @@
         <v>182</v>
       </c>
       <c r="U8" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="W8">
         <v>25</v>
@@ -2391,55 +2403,52 @@
         <v>32.07</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D9" s="29"/>
       <c r="G9" s="26"/>
       <c r="I9" s="26"/>
-      <c r="AC9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D10" s="29"/>
       <c r="G10" s="26"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D11" s="29"/>
       <c r="G11" s="26"/>
       <c r="I11" s="26"/>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D12" s="29"/>
       <c r="G12" s="26"/>
       <c r="I12" s="26"/>
     </row>
-    <row r="13" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="29"/>
       <c r="G13" s="26"/>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D14" s="29"/>
       <c r="G14" s="26"/>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D15" s="29"/>
       <c r="G15" s="26"/>
       <c r="I15" s="26"/>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
       <c r="D16" s="29"/>
       <c r="G16" s="26"/>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D17" s="29"/>
       <c r="G17" s="26"/>
       <c r="I17" s="26"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
       <c r="G18" s="26"/>
       <c r="I18" s="26"/>
     </row>
@@ -2467,14 +2476,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.68359375" customWidth="1"/>
-    <col min="3" max="3" width="49.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="116.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2529,7 +2538,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2551,7 +2560,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2562,7 +2571,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2573,7 +2582,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2584,7 +2593,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2595,7 +2604,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2617,7 +2626,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2625,7 +2634,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2644,7 +2653,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2655,7 +2664,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2663,7 +2672,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2674,7 +2683,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2682,7 +2691,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2693,7 +2702,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2704,7 +2713,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2715,7 +2724,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -2726,7 +2735,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2737,7 +2746,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2748,7 +2757,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -2767,7 +2776,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -2778,7 +2787,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2789,7 +2798,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2833,7 +2842,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2844,7 +2853,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2855,7 +2864,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2863,7 +2872,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2871,7 +2880,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2879,7 +2888,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -2887,7 +2896,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2895,7 +2904,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2903,7 +2912,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2911,7 +2920,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2919,7 +2928,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2927,7 +2936,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2935,7 +2944,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2943,7 +2952,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2951,7 +2960,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2959,7 +2968,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -2978,7 +2987,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -2989,7 +2998,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -3011,7 +3020,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -3022,7 +3031,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3033,7 +3042,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -3044,7 +3053,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -3055,7 +3064,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -3063,7 +3072,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -3071,7 +3080,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -3079,7 +3088,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -3087,7 +3096,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -3095,7 +3104,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -3103,7 +3112,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -3111,7 +3120,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -3119,7 +3128,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -3135,7 +3144,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -3143,7 +3152,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -3151,7 +3160,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -3178,7 +3187,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -3189,7 +3198,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -3200,7 +3209,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -3211,7 +3220,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -3233,7 +3242,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -3257,17 +3266,17 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.26171875" style="25"/>
-    <col min="3" max="3" width="15.41796875" customWidth="1"/>
-    <col min="5" max="5" width="13.26171875" customWidth="1"/>
-    <col min="7" max="7" width="12.26171875" customWidth="1"/>
-    <col min="9" max="9" width="14.26171875" customWidth="1"/>
-    <col min="10" max="10" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="25"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
@@ -3283,7 +3292,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
@@ -3334,14 +3343,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.578125" customWidth="1"/>
-    <col min="3" max="3" width="49.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3363,7 +3372,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3374,7 +3383,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>163</v>
       </c>
@@ -3385,7 +3394,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>164</v>
       </c>
@@ -3396,7 +3405,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>165</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>166</v>
       </c>
@@ -3415,7 +3424,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>167</v>
       </c>
@@ -3426,7 +3435,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>168</v>
       </c>
@@ -3437,7 +3446,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>169</v>
       </c>

</xml_diff>